<commit_message>
aggiornamento Sprint3 nella final Presentation e aggiunta considerazioni nella retrospective
</commit_message>
<xml_diff>
--- a/docs/Sprint 3/Retrospective Report Sprint 3.xlsx
+++ b/docs/Sprint 3/Retrospective Report Sprint 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\Desktop\Sprint 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\IdeaProjects\Progetto-SAD\docs\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FE30214-EAA4-4E00-B961-4E6C923CF262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359D5646-6749-4F10-9949-B0E35742D6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C0809DF1-BB09-4526-AC3F-17FBD68B551A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C0809DF1-BB09-4526-AC3F-17FBD68B551A}"/>
   </bookViews>
   <sheets>
     <sheet name="Starfish diagram" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Sessa Attilio</t>
   </si>
@@ -105,6 +105,14 @@
   </si>
   <si>
     <t>dipendere da strumenti LLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  Creare o mantenere un ambiente di lavoro eccessivamente pressante che possa influenzare negativamente la serenità e la produttività del team.     
+2.eccessivo controllo per ogni dettaglio, a scapito della fiducia nel lavoro svolto dagli altri membri del gruppo.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Prendere decisioni unilaterali sul lavoro da assegnare, senza coinvolgere attivamente tutti i membri del team, limitando l’autonomia e la partecipazione                                                             2. Intervenire sul lavoro altrui senza confronto preventivo, generando confusione e rendendo vani gli sforzi già fatti.                                                      3.Insistere nel voler realizzare funzionalità non previste o non chiaramente definite</t>
   </si>
 </sst>
 </file>
@@ -680,18 +688,18 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="40.81640625" customWidth="1"/>
-    <col min="5" max="5" width="42.453125" customWidth="1"/>
-    <col min="6" max="6" width="40.81640625" customWidth="1"/>
+    <col min="1" max="1" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="40.77734375" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -731,7 +739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="79.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -751,7 +759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="74" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -771,7 +779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="395.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -782,22 +790,22 @@
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="7"/>
     </row>
   </sheetData>
@@ -818,14 +826,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5c58566a-13fc-43ed-a6e6-c82e40767f2f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B6892882E8908E4A901FE9C31570D6B9" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="40616fcd5521fe809d58c1d4145c3584">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5c58566a-13fc-43ed-a6e6-c82e40767f2f" xmlns:ns4="e0abb81f-f5b2-495e-a349-883cf64f59f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed2d4d3cdc0c5f726b3faf01688aa5e5" ns3:_="" ns4:_="">
     <xsd:import namespace="5c58566a-13fc-43ed-a6e6-c82e40767f2f"/>
@@ -1020,6 +1020,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5c58566a-13fc-43ed-a6e6-c82e40767f2f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C30C96D9-B08E-4F5A-B32F-75F5DEE5F04B}">
   <ds:schemaRefs>
@@ -1029,23 +1037,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E361CAB8-D59B-4E57-A535-83A62C5A63A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5c58566a-13fc-43ed-a6e6-c82e40767f2f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="e0abb81f-f5b2-495e-a349-883cf64f59f8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAFE9F65-B046-4CB4-A117-501B197E61A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1062,4 +1053,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E361CAB8-D59B-4E57-A535-83A62C5A63A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5c58566a-13fc-43ed-a6e6-c82e40767f2f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="e0abb81f-f5b2-495e-a349-883cf64f59f8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>